<commit_message>
Updating how thermal threshold is calculated in ectopic expression such that absolute value of response must be at least 3*STD(wt response) above the WT response
</commit_message>
<xml_diff>
--- a/Code/Plotting in R/Data/EctopicExpression_R_Import.xlsx
+++ b/Code/Plotting in R/Data/EctopicExpression_R_Import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Box Sync/Lab_Hallem/Astra/Writing/Bryant et al 20xx/Data/Calcium Imaging/Ectopic Expression/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Documents/RStudio/Bryant_et_al_2021/Code/Plotting in R/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C9AC76-3BD2-E94F-A0D3-5AB0FE70732E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A087F1-DEDE-0347-B195-FD86C60805D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11360" yWindow="640" windowWidth="24680" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3140" yWindow="3460" windowWidth="24680" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="82" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="111" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1588,7 +1588,7 @@
         <v>58</v>
       </c>
       <c r="D43">
-        <v>23.4</v>
+        <v>24</v>
       </c>
       <c r="E43" s="4">
         <v>37.200000000000003</v>
@@ -1605,7 +1605,7 @@
         <v>59</v>
       </c>
       <c r="D44">
-        <v>21.8</v>
+        <v>21.7</v>
       </c>
       <c r="E44" s="4">
         <v>39.9</v>
@@ -1639,7 +1639,7 @@
         <v>61</v>
       </c>
       <c r="D46">
-        <v>39.950000000000003</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="E46" s="4">
         <v>40</v>
@@ -1656,7 +1656,7 @@
         <v>62</v>
       </c>
       <c r="D47">
-        <v>31.6</v>
+        <v>31</v>
       </c>
       <c r="E47" s="4">
         <v>40.200000000000003</v>
@@ -1673,7 +1673,7 @@
         <v>63</v>
       </c>
       <c r="D48">
-        <v>21.8</v>
+        <v>22</v>
       </c>
       <c r="E48" s="4">
         <v>36.200000000000003</v>
@@ -1690,7 +1690,7 @@
         <v>64</v>
       </c>
       <c r="D49">
-        <v>21.5</v>
+        <v>21.6</v>
       </c>
       <c r="E49" s="4">
         <v>40.1</v>
@@ -1707,7 +1707,7 @@
         <v>65</v>
       </c>
       <c r="D50">
-        <v>21.6</v>
+        <v>21.55</v>
       </c>
       <c r="E50" s="4">
         <v>36.299999999999997</v>
@@ -1724,7 +1724,7 @@
         <v>66</v>
       </c>
       <c r="D51">
-        <v>24.1</v>
+        <v>23.9</v>
       </c>
       <c r="E51" s="4">
         <v>36.700000000000003</v>
@@ -1740,12 +1740,6 @@
       <c r="C52" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D52">
-        <v>39.9</v>
-      </c>
-      <c r="E52" s="4">
-        <v>40</v>
-      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
@@ -1775,7 +1769,7 @@
         <v>69</v>
       </c>
       <c r="D54">
-        <v>29.45</v>
+        <v>29.4</v>
       </c>
       <c r="E54" s="4">
         <v>39.5</v>
@@ -1792,7 +1786,7 @@
         <v>70</v>
       </c>
       <c r="D55">
-        <v>27.05</v>
+        <v>27.3</v>
       </c>
       <c r="E55" s="4">
         <v>39.849999999999994</v>

</xml_diff>